<commit_message>
Added date formatting to excel template generation
</commit_message>
<xml_diff>
--- a/data/template.xlsx
+++ b/data/template.xlsx
@@ -9222,6 +9222,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -9292,11 +9295,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -33490,7 +33494,7 @@
   <cols>
     <col min="1" max="1" width="26.7109375" customWidth="1"/>
     <col min="2" max="2" width="42.7109375" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" customWidth="1"/>
+    <col min="3" max="3" width="38.7109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" customWidth="1"/>
     <col min="5" max="5" width="44.7109375" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="36.7109375" hidden="1" customWidth="1"/>
@@ -33520,7 +33524,7 @@
     <col min="33" max="33" width="126.7109375" hidden="1" customWidth="1"/>
     <col min="34" max="34" width="108.7109375" hidden="1" customWidth="1"/>
     <col min="35" max="35" width="104.7109375" hidden="1" customWidth="1"/>
-    <col min="36" max="36" width="60.7109375" hidden="1" customWidth="1"/>
+    <col min="36" max="36" width="60.7109375" style="2" hidden="1" customWidth="1"/>
     <col min="37" max="37" width="84.7109375" customWidth="1"/>
     <col min="38" max="39" width="102.7109375" customWidth="1"/>
     <col min="40" max="40" width="130.7109375" hidden="1" customWidth="1"/>
@@ -33532,7 +33536,7 @@
     <col min="46" max="46" width="148.7109375" hidden="1" customWidth="1"/>
     <col min="47" max="47" width="130.7109375" hidden="1" customWidth="1"/>
     <col min="48" max="48" width="126.7109375" hidden="1" customWidth="1"/>
-    <col min="49" max="49" width="82.7109375" hidden="1" customWidth="1"/>
+    <col min="49" max="49" width="82.7109375" style="2" hidden="1" customWidth="1"/>
     <col min="50" max="50" width="70.7109375" hidden="1" customWidth="1"/>
     <col min="51" max="52" width="88.7109375" hidden="1" customWidth="1"/>
     <col min="53" max="53" width="116.7109375" hidden="1" customWidth="1"/>
@@ -33544,13 +33548,13 @@
     <col min="59" max="59" width="134.7109375" hidden="1" customWidth="1"/>
     <col min="60" max="60" width="116.7109375" hidden="1" customWidth="1"/>
     <col min="61" max="61" width="112.7109375" hidden="1" customWidth="1"/>
-    <col min="62" max="62" width="68.7109375" hidden="1" customWidth="1"/>
+    <col min="62" max="62" width="68.7109375" style="2" hidden="1" customWidth="1"/>
     <col min="63" max="63" width="82.7109375" hidden="1" customWidth="1"/>
     <col min="64" max="64" width="78.7109375" hidden="1" customWidth="1"/>
     <col min="65" max="65" width="12.7109375" hidden="1" customWidth="1"/>
-    <col min="66" max="66" width="40.7109375" hidden="1" customWidth="1"/>
+    <col min="66" max="66" width="40.7109375" style="2" hidden="1" customWidth="1"/>
     <col min="67" max="67" width="30.7109375" hidden="1" customWidth="1"/>
-    <col min="68" max="68" width="24.7109375" hidden="1" customWidth="1"/>
+    <col min="68" max="68" width="24.7109375" style="2" hidden="1" customWidth="1"/>
     <col min="69" max="69" width="60.7109375" hidden="1" customWidth="1"/>
     <col min="70" max="70" width="92.7109375" hidden="1" customWidth="1"/>
     <col min="71" max="71" width="94.7109375" hidden="1" customWidth="1"/>
@@ -33560,7 +33564,7 @@
     <col min="75" max="75" width="78.7109375" hidden="1" customWidth="1"/>
     <col min="76" max="76" width="60.7109375" hidden="1" customWidth="1"/>
     <col min="77" max="77" width="56.7109375" hidden="1" customWidth="1"/>
-    <col min="78" max="78" width="20.7109375" hidden="1" customWidth="1"/>
+    <col min="78" max="78" width="20.7109375" style="2" hidden="1" customWidth="1"/>
     <col min="79" max="79" width="44.7109375" hidden="1" customWidth="1"/>
     <col min="80" max="81" width="58.7109375" hidden="1" customWidth="1"/>
     <col min="82" max="82" width="70.7109375" hidden="1" customWidth="1"/>
@@ -33579,11 +33583,11 @@
     <col min="95" max="95" width="62.7109375" hidden="1" customWidth="1"/>
     <col min="96" max="96" width="44.7109375" hidden="1" customWidth="1"/>
     <col min="97" max="97" width="40.7109375" hidden="1" customWidth="1"/>
-    <col min="98" max="98" width="30.7109375" hidden="1" customWidth="1"/>
+    <col min="98" max="98" width="30.7109375" style="2" hidden="1" customWidth="1"/>
     <col min="99" max="99" width="16.7109375" hidden="1" customWidth="1"/>
     <col min="100" max="100" width="12.7109375" hidden="1" customWidth="1"/>
     <col min="101" max="101" width="26.7109375" hidden="1" customWidth="1"/>
-    <col min="102" max="102" width="44.7109375" hidden="1" customWidth="1"/>
+    <col min="102" max="102" width="44.7109375" style="2" hidden="1" customWidth="1"/>
     <col min="103" max="103" width="42.7109375" hidden="1" customWidth="1"/>
     <col min="104" max="104" width="48.7109375" hidden="1" customWidth="1"/>
     <col min="105" max="105" width="40.7109375" hidden="1" customWidth="1"/>
@@ -33593,16 +33597,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:108" hidden="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -33919,16 +33923,16 @@
       </c>
     </row>
     <row r="2" spans="1:108" hidden="1">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -34065,27 +34069,27 @@
       <c r="DD2" s="1"/>
     </row>
     <row r="3" spans="1:108" hidden="1">
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
       <c r="V3" s="1" t="s">
         <v>42</v>
       </c>
@@ -34141,20 +34145,20 @@
         <v>93</v>
       </c>
       <c r="BL3" s="1"/>
-      <c r="BP3" s="3" t="s">
+      <c r="BP3" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="BQ3" s="3" t="s">
+      <c r="BQ3" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="BR3" s="3"/>
-      <c r="BS3" s="3"/>
-      <c r="BT3" s="3"/>
-      <c r="BU3" s="3"/>
-      <c r="BV3" s="3"/>
-      <c r="BW3" s="3"/>
-      <c r="BX3" s="3"/>
-      <c r="BY3" s="3"/>
+      <c r="BR3" s="4"/>
+      <c r="BS3" s="4"/>
+      <c r="BT3" s="4"/>
+      <c r="BU3" s="4"/>
+      <c r="BV3" s="4"/>
+      <c r="BW3" s="4"/>
+      <c r="BX3" s="4"/>
+      <c r="BY3" s="4"/>
       <c r="BZ3" s="1" t="s">
         <v>111</v>
       </c>
@@ -34181,13 +34185,13 @@
         <v>133</v>
       </c>
       <c r="CK3" s="1"/>
-      <c r="CL3" s="3" t="s">
+      <c r="CL3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="CM3" s="3" t="s">
+      <c r="CM3" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="CN3" s="3" t="s">
+      <c r="CN3" s="4" t="s">
         <v>139</v>
       </c>
       <c r="CO3" s="1" t="s">
@@ -34200,17 +34204,17 @@
       <c r="CT3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="CW3" s="3" t="s">
+      <c r="CW3" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="CX3" s="3" t="s">
+      <c r="CX3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="CY3" s="3"/>
-      <c r="CZ3" s="3" t="s">
+      <c r="CY3" s="4"/>
+      <c r="CZ3" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="DA3" s="3"/>
+      <c r="DA3" s="4"/>
       <c r="DB3" s="1" t="s">
         <v>161</v>
       </c>
@@ -34222,110 +34226,110 @@
       </c>
     </row>
     <row r="4" spans="1:108" hidden="1">
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="M4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="X4" s="3" t="s">
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="X4" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="Y4" s="3" t="s">
+      <c r="Y4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="Z4" s="3" t="s">
+      <c r="Z4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="AA4" s="3" t="s">
+      <c r="AA4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AB4" s="3"/>
-      <c r="AC4" s="3"/>
-      <c r="AD4" s="3"/>
-      <c r="AE4" s="3"/>
-      <c r="AF4" s="3"/>
-      <c r="AG4" s="3"/>
-      <c r="AH4" s="3"/>
-      <c r="AI4" s="3"/>
+      <c r="AB4" s="4"/>
+      <c r="AC4" s="4"/>
+      <c r="AD4" s="4"/>
+      <c r="AE4" s="4"/>
+      <c r="AF4" s="4"/>
+      <c r="AG4" s="4"/>
+      <c r="AH4" s="4"/>
+      <c r="AI4" s="4"/>
       <c r="AJ4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AK4" s="3" t="s">
+      <c r="AK4" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AL4" s="3" t="s">
+      <c r="AL4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AM4" s="3" t="s">
+      <c r="AM4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="AN4" s="3" t="s">
+      <c r="AN4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AO4" s="3"/>
-      <c r="AP4" s="3"/>
-      <c r="AQ4" s="3"/>
-      <c r="AR4" s="3"/>
-      <c r="AS4" s="3"/>
-      <c r="AT4" s="3"/>
-      <c r="AU4" s="3"/>
-      <c r="AV4" s="3"/>
+      <c r="AO4" s="4"/>
+      <c r="AP4" s="4"/>
+      <c r="AQ4" s="4"/>
+      <c r="AR4" s="4"/>
+      <c r="AS4" s="4"/>
+      <c r="AT4" s="4"/>
+      <c r="AU4" s="4"/>
+      <c r="AV4" s="4"/>
       <c r="AW4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AX4" s="3" t="s">
+      <c r="AX4" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AY4" s="3" t="s">
+      <c r="AY4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AZ4" s="3" t="s">
+      <c r="AZ4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="BA4" s="3" t="s">
+      <c r="BA4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="BB4" s="3"/>
-      <c r="BC4" s="3"/>
-      <c r="BD4" s="3"/>
-      <c r="BE4" s="3"/>
-      <c r="BF4" s="3"/>
-      <c r="BG4" s="3"/>
-      <c r="BH4" s="3"/>
-      <c r="BI4" s="3"/>
+      <c r="BB4" s="4"/>
+      <c r="BC4" s="4"/>
+      <c r="BD4" s="4"/>
+      <c r="BE4" s="4"/>
+      <c r="BF4" s="4"/>
+      <c r="BG4" s="4"/>
+      <c r="BH4" s="4"/>
+      <c r="BI4" s="4"/>
       <c r="BJ4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="BK4" s="3" t="s">
+      <c r="BK4" s="4" t="s">
         <v>90</v>
       </c>
       <c r="BL4" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="BQ4" s="3" t="s">
+      <c r="BQ4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="BR4" s="3"/>
-      <c r="BS4" s="3"/>
-      <c r="BT4" s="3"/>
+      <c r="BR4" s="4"/>
+      <c r="BS4" s="4"/>
+      <c r="BT4" s="4"/>
       <c r="BU4" s="1" t="s">
         <v>38</v>
       </c>
@@ -34333,10 +34337,10 @@
       <c r="BW4" s="1"/>
       <c r="BX4" s="1"/>
       <c r="BY4" s="1"/>
-      <c r="CB4" s="3" t="s">
+      <c r="CB4" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="CC4" s="3" t="s">
+      <c r="CC4" s="4" t="s">
         <v>111</v>
       </c>
       <c r="CD4" s="1" t="s">
@@ -34360,7 +34364,7 @@
       <c r="CK4" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="CO4" s="3" t="s">
+      <c r="CO4" s="4" t="s">
         <v>20</v>
       </c>
       <c r="CP4" s="1" t="s">
@@ -34381,20 +34385,20 @@
       <c r="CY4" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="CZ4" s="3" t="s">
+      <c r="CZ4" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="DA4" s="3" t="s">
+      <c r="DA4" s="4" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:108" hidden="1">
-      <c r="M5" s="3" t="s">
+      <c r="M5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
       <c r="Q5" s="1" t="s">
         <v>38</v>
       </c>
@@ -34402,12 +34406,12 @@
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
-      <c r="AA5" s="3" t="s">
+      <c r="AA5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AB5" s="3"/>
-      <c r="AC5" s="3"/>
-      <c r="AD5" s="3"/>
+      <c r="AB5" s="4"/>
+      <c r="AC5" s="4"/>
+      <c r="AD5" s="4"/>
       <c r="AE5" s="1" t="s">
         <v>38</v>
       </c>
@@ -34415,12 +34419,12 @@
       <c r="AG5" s="1"/>
       <c r="AH5" s="1"/>
       <c r="AI5" s="1"/>
-      <c r="AN5" s="3" t="s">
+      <c r="AN5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AO5" s="3"/>
-      <c r="AP5" s="3"/>
-      <c r="AQ5" s="3"/>
+      <c r="AO5" s="4"/>
+      <c r="AP5" s="4"/>
+      <c r="AQ5" s="4"/>
       <c r="AR5" s="1" t="s">
         <v>38</v>
       </c>
@@ -34428,12 +34432,12 @@
       <c r="AT5" s="1"/>
       <c r="AU5" s="1"/>
       <c r="AV5" s="1"/>
-      <c r="BA5" s="3" t="s">
+      <c r="BA5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="BB5" s="3"/>
-      <c r="BC5" s="3"/>
-      <c r="BD5" s="3"/>
+      <c r="BB5" s="4"/>
+      <c r="BC5" s="4"/>
+      <c r="BD5" s="4"/>
       <c r="BE5" s="1" t="s">
         <v>38</v>
       </c>
@@ -34441,15 +34445,15 @@
       <c r="BG5" s="1"/>
       <c r="BH5" s="1"/>
       <c r="BI5" s="1"/>
-      <c r="BQ5" s="3" t="s">
+      <c r="BQ5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="BR5" s="3" t="s">
+      <c r="BR5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="BS5" s="3"/>
-      <c r="BT5" s="3"/>
-      <c r="BU5" s="3" t="s">
+      <c r="BS5" s="4"/>
+      <c r="BT5" s="4"/>
+      <c r="BU5" s="4" t="s">
         <v>20</v>
       </c>
       <c r="BV5" s="1" t="s">
@@ -34466,15 +34470,15 @@
       </c>
     </row>
     <row r="6" spans="1:108" hidden="1">
-      <c r="M6" s="3" t="s">
+      <c r="M6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="N6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3" t="s">
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4" t="s">
         <v>20</v>
       </c>
       <c r="R6" s="1" t="s">
@@ -34489,15 +34493,15 @@
       <c r="U6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AA6" s="3" t="s">
+      <c r="AA6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="AB6" s="3" t="s">
+      <c r="AB6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AC6" s="3"/>
-      <c r="AD6" s="3"/>
-      <c r="AE6" s="3" t="s">
+      <c r="AC6" s="4"/>
+      <c r="AD6" s="4"/>
+      <c r="AE6" s="4" t="s">
         <v>20</v>
       </c>
       <c r="AF6" s="1" t="s">
@@ -34512,15 +34516,15 @@
       <c r="AI6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AN6" s="3" t="s">
+      <c r="AN6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="AO6" s="3" t="s">
+      <c r="AO6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AP6" s="3"/>
-      <c r="AQ6" s="3"/>
-      <c r="AR6" s="3" t="s">
+      <c r="AP6" s="4"/>
+      <c r="AQ6" s="4"/>
+      <c r="AR6" s="4" t="s">
         <v>20</v>
       </c>
       <c r="AS6" s="1" t="s">
@@ -34535,15 +34539,15 @@
       <c r="AV6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="BA6" s="3" t="s">
+      <c r="BA6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="BB6" s="3" t="s">
+      <c r="BB6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="BC6" s="3"/>
-      <c r="BD6" s="3"/>
-      <c r="BE6" s="3" t="s">
+      <c r="BC6" s="4"/>
+      <c r="BD6" s="4"/>
+      <c r="BE6" s="4" t="s">
         <v>20</v>
       </c>
       <c r="BF6" s="1" t="s">
@@ -34558,7 +34562,7 @@
       <c r="BI6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="BR6" s="3" t="s">
+      <c r="BR6" s="4" t="s">
         <v>22</v>
       </c>
       <c r="BS6" s="1" t="s">
@@ -34569,7 +34573,7 @@
       </c>
     </row>
     <row r="7" spans="1:108" hidden="1">
-      <c r="N7" s="3" t="s">
+      <c r="N7" s="4" t="s">
         <v>22</v>
       </c>
       <c r="O7" s="1" t="s">
@@ -34578,7 +34582,7 @@
       <c r="P7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB7" s="3" t="s">
+      <c r="AB7" s="4" t="s">
         <v>22</v>
       </c>
       <c r="AC7" s="1" t="s">
@@ -34587,7 +34591,7 @@
       <c r="AD7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AO7" s="3" t="s">
+      <c r="AO7" s="4" t="s">
         <v>22</v>
       </c>
       <c r="AP7" s="1" t="s">
@@ -34596,7 +34600,7 @@
       <c r="AQ7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="BB7" s="3" t="s">
+      <c r="BB7" s="4" t="s">
         <v>22</v>
       </c>
       <c r="BC7" s="1" t="s">
@@ -34607,16 +34611,16 @@
       </c>
     </row>
     <row r="8" spans="1:108">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -35066,7 +35070,7 @@
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="34.7109375" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="38.7109375" customWidth="1"/>
+    <col min="5" max="5" width="38.7109375" style="2" customWidth="1"/>
     <col min="6" max="6" width="30.7109375" customWidth="1"/>
     <col min="7" max="7" width="28.7109375" customWidth="1"/>
     <col min="8" max="8" width="44.7109375" hidden="1" customWidth="1"/>
@@ -35075,7 +35079,7 @@
     <col min="12" max="12" width="60.7109375" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="44.7109375" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="40.7109375" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="40.7109375" style="2" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="38.7109375" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="34.7109375" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="68.7109375" hidden="1" customWidth="1"/>
@@ -35101,11 +35105,11 @@
     <col min="41" max="41" width="62.7109375" hidden="1" customWidth="1"/>
     <col min="42" max="42" width="44.7109375" hidden="1" customWidth="1"/>
     <col min="43" max="43" width="40.7109375" hidden="1" customWidth="1"/>
-    <col min="44" max="44" width="30.7109375" hidden="1" customWidth="1"/>
+    <col min="44" max="44" width="30.7109375" style="2" hidden="1" customWidth="1"/>
     <col min="45" max="45" width="16.7109375" customWidth="1"/>
     <col min="46" max="46" width="12.7109375" hidden="1" customWidth="1"/>
     <col min="47" max="47" width="26.7109375" hidden="1" customWidth="1"/>
-    <col min="48" max="48" width="44.7109375" hidden="1" customWidth="1"/>
+    <col min="48" max="48" width="44.7109375" style="2" hidden="1" customWidth="1"/>
     <col min="49" max="49" width="42.7109375" hidden="1" customWidth="1"/>
     <col min="50" max="50" width="48.7109375" hidden="1" customWidth="1"/>
     <col min="51" max="51" width="40.7109375" hidden="1" customWidth="1"/>
@@ -35115,25 +35119,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:54" hidden="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>991</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>990</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>992</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>993</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>995</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -35279,30 +35283,30 @@
       </c>
     </row>
     <row r="2" spans="1:54" hidden="1">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>991</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>990</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>992</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>1007</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
       <c r="M2" s="1" t="s">
         <v>8</v>
       </c>
@@ -35371,10 +35375,10 @@
       <c r="BB2" s="1"/>
     </row>
     <row r="3" spans="1:54" hidden="1">
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="4" t="s">
         <v>994</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="4" t="s">
         <v>996</v>
       </c>
       <c r="H3" s="1" t="s">
@@ -35392,7 +35396,7 @@
       <c r="L3" s="1" t="s">
         <v>1006</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="N3" s="1" t="s">
@@ -35425,22 +35429,22 @@
       <c r="AD3" s="1"/>
       <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
-      <c r="AG3" s="3" t="s">
+      <c r="AG3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="AH3" s="3" t="s">
+      <c r="AH3" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="AI3" s="3" t="s">
+      <c r="AI3" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="AJ3" s="3" t="s">
+      <c r="AJ3" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="AK3" s="3" t="s">
+      <c r="AK3" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="AL3" s="3" t="s">
+      <c r="AL3" s="4" t="s">
         <v>139</v>
       </c>
       <c r="AM3" s="1" t="s">
@@ -35453,17 +35457,17 @@
       <c r="AR3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AU3" s="3" t="s">
+      <c r="AU3" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="AV3" s="3" t="s">
+      <c r="AV3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AW3" s="3"/>
-      <c r="AX3" s="3" t="s">
+      <c r="AW3" s="4"/>
+      <c r="AX3" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="AY3" s="3"/>
+      <c r="AY3" s="4"/>
       <c r="AZ3" s="1" t="s">
         <v>161</v>
       </c>
@@ -35475,7 +35479,7 @@
       </c>
     </row>
     <row r="4" spans="1:54" hidden="1">
-      <c r="V4" s="3" t="s">
+      <c r="V4" s="4" t="s">
         <v>20</v>
       </c>
       <c r="W4" s="1" t="s">
@@ -35490,13 +35494,13 @@
       <c r="Z4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AA4" s="3" t="s">
+      <c r="AA4" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="AB4" s="3" t="s">
+      <c r="AB4" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="AC4" s="3" t="s">
+      <c r="AC4" s="4" t="s">
         <v>1028</v>
       </c>
       <c r="AD4" s="1" t="s">
@@ -35508,7 +35512,7 @@
       <c r="AF4" s="1" t="s">
         <v>1033</v>
       </c>
-      <c r="AM4" s="3" t="s">
+      <c r="AM4" s="4" t="s">
         <v>20</v>
       </c>
       <c r="AN4" s="1" t="s">
@@ -35529,33 +35533,33 @@
       <c r="AW4" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="AX4" s="3" t="s">
+      <c r="AX4" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="AY4" s="3" t="s">
+      <c r="AY4" s="4" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:54">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>1043</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>991</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>1051</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>992</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="3" t="s">
         <v>994</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="3" t="s">
         <v>996</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -35795,7 +35799,7 @@
     <col min="1" max="1" width="34.7109375" customWidth="1"/>
     <col min="2" max="2" width="40.7109375" customWidth="1"/>
     <col min="3" max="3" width="34.7109375" customWidth="1"/>
-    <col min="4" max="4" width="40.7109375" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="46.7109375" customWidth="1"/>
     <col min="6" max="6" width="50.7109375" customWidth="1"/>
     <col min="7" max="7" width="44.7109375" hidden="1" customWidth="1"/>
@@ -35805,8 +35809,8 @@
     <col min="11" max="11" width="92.7109375" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="74.7109375" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="70.7109375" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="60.7109375" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="50.7109375" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="60.7109375" style="2" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="50.7109375" style="2" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="54.7109375" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="56.7109375" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="90.7109375" hidden="1" customWidth="1"/>
@@ -35827,8 +35831,8 @@
     <col min="34" max="34" width="102.7109375" hidden="1" customWidth="1"/>
     <col min="35" max="35" width="84.7109375" hidden="1" customWidth="1"/>
     <col min="36" max="36" width="80.7109375" hidden="1" customWidth="1"/>
-    <col min="37" max="37" width="70.7109375" hidden="1" customWidth="1"/>
-    <col min="38" max="38" width="50.7109375" hidden="1" customWidth="1"/>
+    <col min="37" max="37" width="70.7109375" style="2" hidden="1" customWidth="1"/>
+    <col min="38" max="38" width="50.7109375" style="2" hidden="1" customWidth="1"/>
     <col min="39" max="39" width="68.7109375" hidden="1" customWidth="1"/>
     <col min="40" max="40" width="56.7109375" hidden="1" customWidth="1"/>
     <col min="41" max="41" width="64.7109375" hidden="1" customWidth="1"/>
@@ -35843,8 +35847,8 @@
     <col min="50" max="50" width="102.7109375" hidden="1" customWidth="1"/>
     <col min="51" max="51" width="84.7109375" hidden="1" customWidth="1"/>
     <col min="52" max="52" width="80.7109375" hidden="1" customWidth="1"/>
-    <col min="53" max="53" width="70.7109375" hidden="1" customWidth="1"/>
-    <col min="54" max="54" width="66.7109375" hidden="1" customWidth="1"/>
+    <col min="53" max="53" width="70.7109375" style="2" hidden="1" customWidth="1"/>
+    <col min="54" max="54" width="66.7109375" style="2" hidden="1" customWidth="1"/>
     <col min="55" max="55" width="70.7109375" hidden="1" customWidth="1"/>
     <col min="56" max="56" width="72.7109375" hidden="1" customWidth="1"/>
     <col min="57" max="57" width="106.7109375" hidden="1" customWidth="1"/>
@@ -35865,7 +35869,7 @@
     <col min="73" max="73" width="118.7109375" hidden="1" customWidth="1"/>
     <col min="74" max="74" width="100.7109375" hidden="1" customWidth="1"/>
     <col min="75" max="75" width="96.7109375" hidden="1" customWidth="1"/>
-    <col min="76" max="76" width="86.7109375" hidden="1" customWidth="1"/>
+    <col min="76" max="76" width="86.7109375" style="2" hidden="1" customWidth="1"/>
     <col min="77" max="77" width="16.7109375" hidden="1" customWidth="1"/>
     <col min="78" max="80" width="14.7109375" hidden="1" customWidth="1"/>
     <col min="81" max="81" width="52.7109375" customWidth="1"/>
@@ -35886,7 +35890,7 @@
     <col min="96" max="96" width="118.7109375" hidden="1" customWidth="1"/>
     <col min="97" max="97" width="100.7109375" hidden="1" customWidth="1"/>
     <col min="98" max="98" width="96.7109375" hidden="1" customWidth="1"/>
-    <col min="99" max="99" width="60.7109375" customWidth="1"/>
+    <col min="99" max="99" width="60.7109375" style="2" customWidth="1"/>
     <col min="100" max="100" width="58.7109375" hidden="1" customWidth="1"/>
     <col min="101" max="101" width="104.7109375" customWidth="1"/>
     <col min="102" max="102" width="136.7109375" hidden="1" customWidth="1"/>
@@ -35902,7 +35906,7 @@
     <col min="112" max="112" width="118.7109375" hidden="1" customWidth="1"/>
     <col min="113" max="113" width="100.7109375" hidden="1" customWidth="1"/>
     <col min="114" max="114" width="96.7109375" hidden="1" customWidth="1"/>
-    <col min="115" max="115" width="60.7109375" customWidth="1"/>
+    <col min="115" max="115" width="60.7109375" style="2" customWidth="1"/>
     <col min="116" max="116" width="58.7109375" hidden="1" customWidth="1"/>
     <col min="117" max="117" width="56.7109375" hidden="1" customWidth="1"/>
     <col min="118" max="118" width="68.7109375" hidden="1" customWidth="1"/>
@@ -35910,9 +35914,9 @@
     <col min="120" max="120" width="88.7109375" hidden="1" customWidth="1"/>
     <col min="121" max="121" width="70.7109375" hidden="1" customWidth="1"/>
     <col min="122" max="122" width="66.7109375" hidden="1" customWidth="1"/>
-    <col min="123" max="123" width="56.7109375" hidden="1" customWidth="1"/>
+    <col min="123" max="123" width="56.7109375" style="2" hidden="1" customWidth="1"/>
     <col min="124" max="124" width="52.7109375" hidden="1" customWidth="1"/>
-    <col min="125" max="125" width="70.7109375" hidden="1" customWidth="1"/>
+    <col min="125" max="125" width="70.7109375" style="2" hidden="1" customWidth="1"/>
     <col min="126" max="126" width="68.7109375" hidden="1" customWidth="1"/>
     <col min="127" max="127" width="74.7109375" hidden="1" customWidth="1"/>
     <col min="128" max="128" width="66.7109375" hidden="1" customWidth="1"/>
@@ -35943,7 +35947,7 @@
     <col min="155" max="155" width="110.7109375" hidden="1" customWidth="1"/>
     <col min="156" max="156" width="92.7109375" hidden="1" customWidth="1"/>
     <col min="157" max="157" width="88.7109375" hidden="1" customWidth="1"/>
-    <col min="158" max="158" width="78.7109375" hidden="1" customWidth="1"/>
+    <col min="158" max="158" width="78.7109375" style="2" hidden="1" customWidth="1"/>
     <col min="159" max="159" width="64.7109375" hidden="1" customWidth="1"/>
     <col min="160" max="160" width="92.7109375" hidden="1" customWidth="1"/>
     <col min="161" max="161" width="84.7109375" hidden="1" customWidth="1"/>
@@ -35965,23 +35969,24 @@
     <col min="178" max="178" width="118.7109375" hidden="1" customWidth="1"/>
     <col min="179" max="179" width="100.7109375" hidden="1" customWidth="1"/>
     <col min="180" max="180" width="96.7109375" hidden="1" customWidth="1"/>
-    <col min="181" max="181" width="60.7109375" hidden="1" customWidth="1"/>
+    <col min="181" max="181" width="60.7109375" style="2" hidden="1" customWidth="1"/>
     <col min="182" max="183" width="58.7109375" hidden="1" customWidth="1"/>
     <col min="184" max="184" width="66.7109375" hidden="1" customWidth="1"/>
-    <col min="185" max="187" width="34.7109375" hidden="1" customWidth="1"/>
+    <col min="185" max="185" width="34.7109375" hidden="1" customWidth="1"/>
+    <col min="186" max="187" width="34.7109375" style="2" hidden="1" customWidth="1"/>
     <col min="188" max="188" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="189" max="189" width="54.7109375" hidden="1" customWidth="1"/>
     <col min="190" max="191" width="32.7109375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:191" hidden="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>990</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1564</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>1565</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -36550,13 +36555,13 @@
       </c>
     </row>
     <row r="2" spans="1:191" hidden="1">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>990</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>1546</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="4"/>
       <c r="D2" s="1" t="s">
         <v>1580</v>
       </c>
@@ -36757,19 +36762,19 @@
       <c r="GI2" s="1"/>
     </row>
     <row r="3" spans="1:191" hidden="1">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>991</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>1568</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="4" t="s">
         <v>1570</v>
       </c>
       <c r="G3" s="1" t="s">
@@ -36852,7 +36857,7 @@
       <c r="BV3" s="1"/>
       <c r="BW3" s="1"/>
       <c r="BX3" s="1"/>
-      <c r="BY3" s="3" t="s">
+      <c r="BY3" s="4" t="s">
         <v>154</v>
       </c>
       <c r="BZ3" s="1" t="s">
@@ -36864,7 +36869,7 @@
       <c r="CB3" s="1" t="s">
         <v>1661</v>
       </c>
-      <c r="CC3" s="3" t="s">
+      <c r="CC3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="CD3" s="1" t="s">
@@ -36997,13 +37002,13 @@
       <c r="GC3" s="1" t="s">
         <v>1604</v>
       </c>
-      <c r="GD3" s="3" t="s">
+      <c r="GD3" s="4" t="s">
         <v>1799</v>
       </c>
-      <c r="GE3" s="3" t="s">
+      <c r="GE3" s="4" t="s">
         <v>1801</v>
       </c>
-      <c r="GF3" s="3" t="s">
+      <c r="GF3" s="4" t="s">
         <v>1803</v>
       </c>
       <c r="GG3" s="1" t="s">
@@ -37017,7 +37022,7 @@
       </c>
     </row>
     <row r="4" spans="1:191" hidden="1">
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="4" t="s">
         <v>139</v>
       </c>
       <c r="I4" s="1" t="s">
@@ -37030,10 +37035,10 @@
       <c r="N4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="O4" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="P4" s="4" t="s">
         <v>1572</v>
       </c>
       <c r="Q4" s="1" t="s">
@@ -37079,10 +37084,10 @@
       <c r="AI4" s="1"/>
       <c r="AJ4" s="1"/>
       <c r="AK4" s="1"/>
-      <c r="AL4" s="3" t="s">
+      <c r="AL4" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="AM4" s="3" t="s">
+      <c r="AM4" s="4" t="s">
         <v>1615</v>
       </c>
       <c r="AN4" s="1" t="s">
@@ -37107,10 +37112,10 @@
       <c r="AY4" s="1"/>
       <c r="AZ4" s="1"/>
       <c r="BA4" s="1"/>
-      <c r="BB4" s="3" t="s">
+      <c r="BB4" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="BC4" s="3" t="s">
+      <c r="BC4" s="4" t="s">
         <v>1572</v>
       </c>
       <c r="BD4" s="1" t="s">
@@ -37156,57 +37161,57 @@
       <c r="BV4" s="1"/>
       <c r="BW4" s="1"/>
       <c r="BX4" s="1"/>
-      <c r="CD4" s="3" t="s">
+      <c r="CD4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="CE4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="CG4" s="3" t="s">
+      <c r="CG4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="CH4" s="3"/>
-      <c r="CI4" s="3"/>
-      <c r="CJ4" s="3"/>
-      <c r="CK4" s="3"/>
-      <c r="CL4" s="3"/>
-      <c r="CM4" s="3"/>
-      <c r="CN4" s="3"/>
-      <c r="CO4" s="3"/>
-      <c r="CP4" s="3"/>
-      <c r="CQ4" s="3"/>
-      <c r="CR4" s="3"/>
-      <c r="CS4" s="3"/>
-      <c r="CT4" s="3"/>
+      <c r="CH4" s="4"/>
+      <c r="CI4" s="4"/>
+      <c r="CJ4" s="4"/>
+      <c r="CK4" s="4"/>
+      <c r="CL4" s="4"/>
+      <c r="CM4" s="4"/>
+      <c r="CN4" s="4"/>
+      <c r="CO4" s="4"/>
+      <c r="CP4" s="4"/>
+      <c r="CQ4" s="4"/>
+      <c r="CR4" s="4"/>
+      <c r="CS4" s="4"/>
+      <c r="CT4" s="4"/>
       <c r="CU4" s="1" t="s">
         <v>59</v>
       </c>
       <c r="CV4" s="1" t="s">
         <v>1685</v>
       </c>
-      <c r="CW4" s="3" t="s">
+      <c r="CW4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="CX4" s="3"/>
-      <c r="CY4" s="3"/>
-      <c r="CZ4" s="3"/>
-      <c r="DA4" s="3"/>
-      <c r="DB4" s="3"/>
-      <c r="DC4" s="3"/>
-      <c r="DD4" s="3"/>
-      <c r="DE4" s="3"/>
-      <c r="DF4" s="3"/>
-      <c r="DG4" s="3"/>
-      <c r="DH4" s="3"/>
-      <c r="DI4" s="3"/>
-      <c r="DJ4" s="3"/>
+      <c r="CX4" s="4"/>
+      <c r="CY4" s="4"/>
+      <c r="CZ4" s="4"/>
+      <c r="DA4" s="4"/>
+      <c r="DB4" s="4"/>
+      <c r="DC4" s="4"/>
+      <c r="DD4" s="4"/>
+      <c r="DE4" s="4"/>
+      <c r="DF4" s="4"/>
+      <c r="DG4" s="4"/>
+      <c r="DH4" s="4"/>
+      <c r="DI4" s="4"/>
+      <c r="DJ4" s="4"/>
       <c r="DK4" s="1" t="s">
         <v>59</v>
       </c>
       <c r="DL4" s="1" t="s">
         <v>1685</v>
       </c>
-      <c r="DM4" s="3" t="s">
+      <c r="DM4" s="4" t="s">
         <v>139</v>
       </c>
       <c r="DN4" s="1" t="s">
@@ -37219,17 +37224,17 @@
       <c r="DS4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="DT4" s="3" t="s">
+      <c r="DT4" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="DU4" s="3" t="s">
+      <c r="DU4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="DV4" s="3"/>
-      <c r="DW4" s="3" t="s">
+      <c r="DV4" s="4"/>
+      <c r="DW4" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="DX4" s="3"/>
+      <c r="DX4" s="4"/>
       <c r="DY4" s="1" t="s">
         <v>161</v>
       </c>
@@ -37239,14 +37244,14 @@
       <c r="EA4" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="EB4" s="3" t="s">
+      <c r="EB4" s="4" t="s">
         <v>1720</v>
       </c>
-      <c r="EC4" s="3" t="s">
+      <c r="EC4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="ED4" s="3"/>
-      <c r="EE4" s="3" t="s">
+      <c r="ED4" s="4"/>
+      <c r="EE4" s="4" t="s">
         <v>1726</v>
       </c>
       <c r="EF4" s="1" t="s">
@@ -37307,37 +37312,37 @@
       <c r="FG4" s="1" t="s">
         <v>1768</v>
       </c>
-      <c r="FK4" s="3" t="s">
+      <c r="FK4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="FL4" s="3"/>
-      <c r="FM4" s="3"/>
-      <c r="FN4" s="3"/>
-      <c r="FO4" s="3"/>
-      <c r="FP4" s="3"/>
-      <c r="FQ4" s="3"/>
-      <c r="FR4" s="3"/>
-      <c r="FS4" s="3"/>
-      <c r="FT4" s="3"/>
-      <c r="FU4" s="3"/>
-      <c r="FV4" s="3"/>
-      <c r="FW4" s="3"/>
-      <c r="FX4" s="3"/>
+      <c r="FL4" s="4"/>
+      <c r="FM4" s="4"/>
+      <c r="FN4" s="4"/>
+      <c r="FO4" s="4"/>
+      <c r="FP4" s="4"/>
+      <c r="FQ4" s="4"/>
+      <c r="FR4" s="4"/>
+      <c r="FS4" s="4"/>
+      <c r="FT4" s="4"/>
+      <c r="FU4" s="4"/>
+      <c r="FV4" s="4"/>
+      <c r="FW4" s="4"/>
+      <c r="FX4" s="4"/>
       <c r="FY4" s="1" t="s">
         <v>59</v>
       </c>
       <c r="FZ4" s="1" t="s">
         <v>1685</v>
       </c>
-      <c r="GA4" s="3" t="s">
+      <c r="GA4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="GB4" s="3" t="s">
+      <c r="GB4" s="4" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:191" hidden="1">
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="4" t="s">
         <v>20</v>
       </c>
       <c r="J5" s="1" t="s">
@@ -37352,7 +37357,7 @@
       <c r="M5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="V5" s="3" t="s">
+      <c r="V5" s="4" t="s">
         <v>20</v>
       </c>
       <c r="W5" s="1" t="s">
@@ -37367,7 +37372,7 @@
       <c r="Z5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AE5" s="3" t="s">
+      <c r="AE5" s="4" t="s">
         <v>139</v>
       </c>
       <c r="AF5" s="1" t="s">
@@ -37380,7 +37385,7 @@
       <c r="AK5" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AO5" s="3" t="s">
+      <c r="AO5" s="4" t="s">
         <v>20</v>
       </c>
       <c r="AP5" s="1" t="s">
@@ -37395,7 +37400,7 @@
       <c r="AS5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AU5" s="3" t="s">
+      <c r="AU5" s="4" t="s">
         <v>139</v>
       </c>
       <c r="AV5" s="1" t="s">
@@ -37408,7 +37413,7 @@
       <c r="BA5" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="BI5" s="3" t="s">
+      <c r="BI5" s="4" t="s">
         <v>20</v>
       </c>
       <c r="BJ5" s="1" t="s">
@@ -37423,7 +37428,7 @@
       <c r="BM5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="BR5" s="3" t="s">
+      <c r="BR5" s="4" t="s">
         <v>139</v>
       </c>
       <c r="BS5" s="1" t="s">
@@ -37436,43 +37441,43 @@
       <c r="BX5" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="CG5" s="3" t="s">
+      <c r="CG5" s="4" t="s">
         <v>1676</v>
       </c>
-      <c r="CH5" s="3"/>
-      <c r="CI5" s="3"/>
-      <c r="CJ5" s="3"/>
-      <c r="CK5" s="3"/>
-      <c r="CL5" s="3"/>
-      <c r="CM5" s="3"/>
-      <c r="CN5" s="3"/>
-      <c r="CO5" s="3"/>
-      <c r="CP5" s="3" t="s">
+      <c r="CH5" s="4"/>
+      <c r="CI5" s="4"/>
+      <c r="CJ5" s="4"/>
+      <c r="CK5" s="4"/>
+      <c r="CL5" s="4"/>
+      <c r="CM5" s="4"/>
+      <c r="CN5" s="4"/>
+      <c r="CO5" s="4"/>
+      <c r="CP5" s="4" t="s">
         <v>1682</v>
       </c>
-      <c r="CQ5" s="3"/>
-      <c r="CR5" s="3"/>
-      <c r="CS5" s="3"/>
-      <c r="CT5" s="3"/>
-      <c r="CW5" s="3" t="s">
+      <c r="CQ5" s="4"/>
+      <c r="CR5" s="4"/>
+      <c r="CS5" s="4"/>
+      <c r="CT5" s="4"/>
+      <c r="CW5" s="4" t="s">
         <v>1676</v>
       </c>
-      <c r="CX5" s="3"/>
-      <c r="CY5" s="3"/>
-      <c r="CZ5" s="3"/>
-      <c r="DA5" s="3"/>
-      <c r="DB5" s="3"/>
-      <c r="DC5" s="3"/>
-      <c r="DD5" s="3"/>
-      <c r="DE5" s="3"/>
-      <c r="DF5" s="3" t="s">
+      <c r="CX5" s="4"/>
+      <c r="CY5" s="4"/>
+      <c r="CZ5" s="4"/>
+      <c r="DA5" s="4"/>
+      <c r="DB5" s="4"/>
+      <c r="DC5" s="4"/>
+      <c r="DD5" s="4"/>
+      <c r="DE5" s="4"/>
+      <c r="DF5" s="4" t="s">
         <v>1682</v>
       </c>
-      <c r="DG5" s="3"/>
-      <c r="DH5" s="3"/>
-      <c r="DI5" s="3"/>
-      <c r="DJ5" s="3"/>
-      <c r="DN5" s="3" t="s">
+      <c r="DG5" s="4"/>
+      <c r="DH5" s="4"/>
+      <c r="DI5" s="4"/>
+      <c r="DJ5" s="4"/>
+      <c r="DN5" s="4" t="s">
         <v>20</v>
       </c>
       <c r="DO5" s="1" t="s">
@@ -37493,16 +37498,16 @@
       <c r="DV5" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="DW5" s="3" t="s">
+      <c r="DW5" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="DX5" s="3" t="s">
+      <c r="DX5" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="EC5" s="3" t="s">
+      <c r="EC5" s="4" t="s">
         <v>1722</v>
       </c>
-      <c r="ED5" s="3" t="s">
+      <c r="ED5" s="4" t="s">
         <v>1724</v>
       </c>
       <c r="EN5" s="1" t="s">
@@ -37517,17 +37522,17 @@
       <c r="EQ5" s="1" t="s">
         <v>1748</v>
       </c>
-      <c r="ER5" s="3" t="s">
+      <c r="ER5" s="4" t="s">
         <v>1720</v>
       </c>
-      <c r="ES5" s="3" t="s">
+      <c r="ES5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="ET5" s="3"/>
+      <c r="ET5" s="4"/>
       <c r="EU5" s="1" t="s">
         <v>1726</v>
       </c>
-      <c r="EV5" s="3" t="s">
+      <c r="EV5" s="4" t="s">
         <v>139</v>
       </c>
       <c r="EW5" s="1" t="s">
@@ -37540,33 +37545,33 @@
       <c r="FB5" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="FD5" s="3" t="s">
+      <c r="FD5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="FE5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="FK5" s="3" t="s">
+      <c r="FK5" s="4" t="s">
         <v>1676</v>
       </c>
-      <c r="FL5" s="3"/>
-      <c r="FM5" s="3"/>
-      <c r="FN5" s="3"/>
-      <c r="FO5" s="3"/>
-      <c r="FP5" s="3"/>
-      <c r="FQ5" s="3"/>
-      <c r="FR5" s="3"/>
-      <c r="FS5" s="3"/>
-      <c r="FT5" s="3" t="s">
+      <c r="FL5" s="4"/>
+      <c r="FM5" s="4"/>
+      <c r="FN5" s="4"/>
+      <c r="FO5" s="4"/>
+      <c r="FP5" s="4"/>
+      <c r="FQ5" s="4"/>
+      <c r="FR5" s="4"/>
+      <c r="FS5" s="4"/>
+      <c r="FT5" s="4" t="s">
         <v>1682</v>
       </c>
-      <c r="FU5" s="3"/>
-      <c r="FV5" s="3"/>
-      <c r="FW5" s="3"/>
-      <c r="FX5" s="3"/>
+      <c r="FU5" s="4"/>
+      <c r="FV5" s="4"/>
+      <c r="FW5" s="4"/>
+      <c r="FX5" s="4"/>
     </row>
     <row r="6" spans="1:191" hidden="1">
-      <c r="AF6" s="3" t="s">
+      <c r="AF6" s="4" t="s">
         <v>20</v>
       </c>
       <c r="AG6" s="1" t="s">
@@ -37581,7 +37586,7 @@
       <c r="AJ6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AV6" s="3" t="s">
+      <c r="AV6" s="4" t="s">
         <v>20</v>
       </c>
       <c r="AW6" s="1" t="s">
@@ -37596,7 +37601,7 @@
       <c r="AZ6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="BS6" s="3" t="s">
+      <c r="BS6" s="4" t="s">
         <v>20</v>
       </c>
       <c r="BT6" s="1" t="s">
@@ -37611,12 +37616,12 @@
       <c r="BW6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="CG6" s="3" t="s">
+      <c r="CG6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="CH6" s="3"/>
-      <c r="CI6" s="3"/>
-      <c r="CJ6" s="3"/>
+      <c r="CH6" s="4"/>
+      <c r="CI6" s="4"/>
+      <c r="CJ6" s="4"/>
       <c r="CK6" s="1" t="s">
         <v>38</v>
       </c>
@@ -37624,7 +37629,7 @@
       <c r="CM6" s="1"/>
       <c r="CN6" s="1"/>
       <c r="CO6" s="1"/>
-      <c r="CP6" s="3" t="s">
+      <c r="CP6" s="4" t="s">
         <v>20</v>
       </c>
       <c r="CQ6" s="1" t="s">
@@ -37639,12 +37644,12 @@
       <c r="CT6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="CW6" s="3" t="s">
+      <c r="CW6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="CX6" s="3"/>
-      <c r="CY6" s="3"/>
-      <c r="CZ6" s="3"/>
+      <c r="CX6" s="4"/>
+      <c r="CY6" s="4"/>
+      <c r="CZ6" s="4"/>
       <c r="DA6" s="1" t="s">
         <v>38</v>
       </c>
@@ -37652,7 +37657,7 @@
       <c r="DC6" s="1"/>
       <c r="DD6" s="1"/>
       <c r="DE6" s="1"/>
-      <c r="DF6" s="3" t="s">
+      <c r="DF6" s="4" t="s">
         <v>20</v>
       </c>
       <c r="DG6" s="1" t="s">
@@ -37667,13 +37672,13 @@
       <c r="DJ6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="ES6" s="3" t="s">
+      <c r="ES6" s="4" t="s">
         <v>1722</v>
       </c>
-      <c r="ET6" s="3" t="s">
+      <c r="ET6" s="4" t="s">
         <v>1724</v>
       </c>
-      <c r="EW6" s="3" t="s">
+      <c r="EW6" s="4" t="s">
         <v>20</v>
       </c>
       <c r="EX6" s="1" t="s">
@@ -37688,12 +37693,12 @@
       <c r="FA6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="FK6" s="3" t="s">
+      <c r="FK6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="FL6" s="3"/>
-      <c r="FM6" s="3"/>
-      <c r="FN6" s="3"/>
+      <c r="FL6" s="4"/>
+      <c r="FM6" s="4"/>
+      <c r="FN6" s="4"/>
       <c r="FO6" s="1" t="s">
         <v>38</v>
       </c>
@@ -37701,7 +37706,7 @@
       <c r="FQ6" s="1"/>
       <c r="FR6" s="1"/>
       <c r="FS6" s="1"/>
-      <c r="FT6" s="3" t="s">
+      <c r="FT6" s="4" t="s">
         <v>20</v>
       </c>
       <c r="FU6" s="1" t="s">
@@ -37718,15 +37723,15 @@
       </c>
     </row>
     <row r="7" spans="1:191" hidden="1">
-      <c r="CG7" s="3" t="s">
+      <c r="CG7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="CH7" s="3" t="s">
+      <c r="CH7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="CI7" s="3"/>
-      <c r="CJ7" s="3"/>
-      <c r="CK7" s="3" t="s">
+      <c r="CI7" s="4"/>
+      <c r="CJ7" s="4"/>
+      <c r="CK7" s="4" t="s">
         <v>20</v>
       </c>
       <c r="CL7" s="1" t="s">
@@ -37741,15 +37746,15 @@
       <c r="CO7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="CW7" s="3" t="s">
+      <c r="CW7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="CX7" s="3" t="s">
+      <c r="CX7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="CY7" s="3"/>
-      <c r="CZ7" s="3"/>
-      <c r="DA7" s="3" t="s">
+      <c r="CY7" s="4"/>
+      <c r="CZ7" s="4"/>
+      <c r="DA7" s="4" t="s">
         <v>20</v>
       </c>
       <c r="DB7" s="1" t="s">
@@ -37764,15 +37769,15 @@
       <c r="DE7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="FK7" s="3" t="s">
+      <c r="FK7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="FL7" s="3" t="s">
+      <c r="FL7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="FM7" s="3"/>
-      <c r="FN7" s="3"/>
-      <c r="FO7" s="3" t="s">
+      <c r="FM7" s="4"/>
+      <c r="FN7" s="4"/>
+      <c r="FO7" s="4" t="s">
         <v>20</v>
       </c>
       <c r="FP7" s="1" t="s">
@@ -37789,7 +37794,7 @@
       </c>
     </row>
     <row r="8" spans="1:191" hidden="1">
-      <c r="CH8" s="3" t="s">
+      <c r="CH8" s="4" t="s">
         <v>22</v>
       </c>
       <c r="CI8" s="1" t="s">
@@ -37798,7 +37803,7 @@
       <c r="CJ8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="CX8" s="3" t="s">
+      <c r="CX8" s="4" t="s">
         <v>22</v>
       </c>
       <c r="CY8" s="1" t="s">
@@ -37807,7 +37812,7 @@
       <c r="CZ8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="FL8" s="3" t="s">
+      <c r="FL8" s="4" t="s">
         <v>22</v>
       </c>
       <c r="FM8" s="1" t="s">
@@ -37818,13 +37823,13 @@
       </c>
     </row>
     <row r="9" spans="1:191">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>1051</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>1043</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>991</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -38610,8 +38615,8 @@
     <col min="29" max="29" width="76.7109375" hidden="1" customWidth="1"/>
     <col min="30" max="30" width="58.7109375" hidden="1" customWidth="1"/>
     <col min="31" max="31" width="54.7109375" hidden="1" customWidth="1"/>
-    <col min="32" max="32" width="20.7109375" hidden="1" customWidth="1"/>
-    <col min="33" max="33" width="18.7109375" customWidth="1"/>
+    <col min="32" max="32" width="20.7109375" style="2" hidden="1" customWidth="1"/>
+    <col min="33" max="33" width="18.7109375" style="2" customWidth="1"/>
     <col min="34" max="34" width="52.7109375" customWidth="1"/>
     <col min="35" max="35" width="22.7109375" customWidth="1"/>
     <col min="36" max="36" width="12.7109375" hidden="1" customWidth="1"/>
@@ -38625,9 +38630,9 @@
     <col min="44" max="44" width="62.7109375" hidden="1" customWidth="1"/>
     <col min="45" max="45" width="44.7109375" hidden="1" customWidth="1"/>
     <col min="46" max="46" width="40.7109375" hidden="1" customWidth="1"/>
-    <col min="47" max="47" width="30.7109375" hidden="1" customWidth="1"/>
+    <col min="47" max="47" width="30.7109375" style="2" hidden="1" customWidth="1"/>
     <col min="48" max="48" width="26.7109375" hidden="1" customWidth="1"/>
-    <col min="49" max="49" width="44.7109375" hidden="1" customWidth="1"/>
+    <col min="49" max="49" width="44.7109375" style="2" hidden="1" customWidth="1"/>
     <col min="50" max="50" width="42.7109375" hidden="1" customWidth="1"/>
     <col min="51" max="51" width="48.7109375" hidden="1" customWidth="1"/>
     <col min="52" max="52" width="40.7109375" hidden="1" customWidth="1"/>
@@ -38637,13 +38642,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:55" hidden="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>2985</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>2986</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -38667,10 +38672,10 @@
       <c r="J1" s="1" t="s">
         <v>2993</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>2995</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="5" t="s">
         <v>2996</v>
       </c>
       <c r="M1" s="1" t="s">
@@ -38804,31 +38809,31 @@
       </c>
     </row>
     <row r="2" spans="1:55" hidden="1">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>2994</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4" t="s">
         <v>3004</v>
       </c>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
       <c r="T2" s="1" t="s">
         <v>8</v>
       </c>
@@ -38889,12 +38894,12 @@
       <c r="BC2" s="1"/>
     </row>
     <row r="3" spans="1:55" hidden="1">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
       <c r="F3" s="1" t="s">
         <v>38</v>
       </c>
@@ -38902,12 +38907,12 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
       <c r="O3" s="1" t="s">
         <v>38</v>
       </c>
@@ -38915,18 +38920,18 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
-      <c r="T3" s="3" t="s">
+      <c r="T3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="U3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="W3" s="3" t="s">
+      <c r="W3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="X3" s="3"/>
-      <c r="Y3" s="3"/>
-      <c r="Z3" s="3"/>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="4"/>
+      <c r="Z3" s="4"/>
       <c r="AA3" s="1" t="s">
         <v>38</v>
       </c>
@@ -38934,10 +38939,10 @@
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
       <c r="AE3" s="1"/>
-      <c r="AH3" s="3" t="s">
+      <c r="AH3" s="4" t="s">
         <v>3019</v>
       </c>
-      <c r="AI3" s="3" t="s">
+      <c r="AI3" s="4" t="s">
         <v>3021</v>
       </c>
       <c r="AK3" s="1" t="s">
@@ -38949,7 +38954,7 @@
       <c r="AM3" s="1" t="s">
         <v>3028</v>
       </c>
-      <c r="AO3" s="3" t="s">
+      <c r="AO3" s="4" t="s">
         <v>139</v>
       </c>
       <c r="AP3" s="1" t="s">
@@ -38962,17 +38967,17 @@
       <c r="AU3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AV3" s="3" t="s">
+      <c r="AV3" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="AW3" s="3" t="s">
+      <c r="AW3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AX3" s="3"/>
-      <c r="AY3" s="3" t="s">
+      <c r="AX3" s="4"/>
+      <c r="AY3" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="AZ3" s="3"/>
+      <c r="AZ3" s="4"/>
       <c r="BA3" s="1" t="s">
         <v>161</v>
       </c>
@@ -38984,15 +38989,15 @@
       </c>
     </row>
     <row r="4" spans="1:55" hidden="1">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3" t="s">
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4" t="s">
         <v>20</v>
       </c>
       <c r="G4" s="1" t="s">
@@ -39007,15 +39012,15 @@
       <c r="J4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3" t="s">
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4" t="s">
         <v>20</v>
       </c>
       <c r="P4" s="1" t="s">
@@ -39030,15 +39035,15 @@
       <c r="S4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="W4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="X4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="3" t="s">
+      <c r="Y4" s="4"/>
+      <c r="Z4" s="4"/>
+      <c r="AA4" s="4" t="s">
         <v>20</v>
       </c>
       <c r="AB4" s="1" t="s">
@@ -39053,7 +39058,7 @@
       <c r="AE4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AP4" s="3" t="s">
+      <c r="AP4" s="4" t="s">
         <v>20</v>
       </c>
       <c r="AQ4" s="1" t="s">
@@ -39074,15 +39079,15 @@
       <c r="AX4" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="AY4" s="3" t="s">
+      <c r="AY4" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="AZ4" s="3" t="s">
+      <c r="AZ4" s="4" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:55" hidden="1">
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -39091,7 +39096,7 @@
       <c r="E5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L5" s="3" t="s">
+      <c r="L5" s="4" t="s">
         <v>22</v>
       </c>
       <c r="M5" s="1" t="s">
@@ -39100,7 +39105,7 @@
       <c r="N5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="X5" s="3" t="s">
+      <c r="X5" s="4" t="s">
         <v>22</v>
       </c>
       <c r="Y5" s="1" t="s">
@@ -39111,13 +39116,13 @@
       </c>
     </row>
     <row r="6" spans="1:55">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>2994</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>2986</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -39141,10 +39146,10 @@
       <c r="J6" s="1" t="s">
         <v>2993</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="K6" s="5" t="s">
         <v>3004</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="L6" s="5" t="s">
         <v>2996</v>
       </c>
       <c r="M6" s="1" t="s">

</xml_diff>